<commit_message>
Modified Helper Methods in WebAPI + 9 Test Cases Done - Trip Advisor (Owners Page)
</commit_message>
<xml_diff>
--- a/tripAdvisor/src/main/resources/TripAdvisor_OwnersPage_ExpectedElements.xlsx
+++ b/tripAdvisor/src/main/resources/TripAdvisor_OwnersPage_ExpectedElements.xlsx
@@ -9,10 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="7" activeTab="9"/>
   </bookViews>
   <sheets>
-    <sheet name="OwnersPage URL" sheetId="1" r:id="rId1"/>
+    <sheet name="HeaderBar ButtonNames" sheetId="1" r:id="rId1"/>
+    <sheet name="HeaderBar DropdownNames" sheetId="2" r:id="rId2"/>
+    <sheet name="ProductsDropdown Names" sheetId="7" r:id="rId3"/>
+    <sheet name="ProductsDropdown URLs" sheetId="3" r:id="rId4"/>
+    <sheet name="ReviewsDropdown Names" sheetId="8" r:id="rId5"/>
+    <sheet name="ReviewsDropdown URLs" sheetId="4" r:id="rId6"/>
+    <sheet name="MktgToolsDropdown Names" sheetId="9" r:id="rId7"/>
+    <sheet name="MktgToolsDropdown URLs" sheetId="5" r:id="rId8"/>
+    <sheet name="HelpDropdown Names" sheetId="10" r:id="rId9"/>
+    <sheet name="HelpDropdown URLs" sheetId="6" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,9 +33,102 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>https://www.tripadvisor.com/Owners</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+  <si>
+    <t>Claim Your Listing</t>
+  </si>
+  <si>
+    <t>Sign in</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>Reviews</t>
+  </si>
+  <si>
+    <t>Marketing Tools</t>
+  </si>
+  <si>
+    <t>Help</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/business/businessadvantage</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/business/sponsored-placements</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/InstantBooking</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/ForRestaurants/ta_premium</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/ForRestaurants/ta_ads</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/ReviewExpress</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/StickerRequest</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/PromoTools</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/Widgets</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/RegistrationController?flow=core_combined&amp;pid=39538&amp;returnTo=%2FBillingAndPayments&amp;fullscreen=true&amp;requireSecure=true</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisorsupport.com/hc/en-us</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/TripAdvisorInsights</t>
+  </si>
+  <si>
+    <t>https://www.tripadvisor.com/ShowForum-g1-i14281-Owners.html</t>
+  </si>
+  <si>
+    <t>Business Advantage</t>
+  </si>
+  <si>
+    <t>Sponsored Placements</t>
+  </si>
+  <si>
+    <t>Instant Booking</t>
+  </si>
+  <si>
+    <t>Premium for Restaurants</t>
+  </si>
+  <si>
+    <t>Ads for Restaurants</t>
+  </si>
+  <si>
+    <t>Get More Reviews</t>
+  </si>
+  <si>
+    <t>Order Stickers</t>
+  </si>
+  <si>
+    <t>Promotional Tools</t>
+  </si>
+  <si>
+    <t>Website Widgets</t>
+  </si>
+  <si>
+    <t>Billing and Payments</t>
+  </si>
+  <si>
+    <t>Help Center</t>
+  </si>
+  <si>
+    <t>Tripadvisor Best Practices</t>
+  </si>
+  <si>
+    <t>Owners' Forum</t>
   </si>
 </sst>
 </file>
@@ -344,18 +446,321 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="147.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="54.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="35.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
12 Cases - TripAdvisor Owners Page
</commit_message>
<xml_diff>
--- a/tripAdvisor/src/main/resources/TripAdvisor_OwnersPage_ExpectedElements.xlsx
+++ b/tripAdvisor/src/main/resources/TripAdvisor_OwnersPage_ExpectedElements.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" firstSheet="7" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" tabRatio="684" firstSheet="9" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="HeaderBar ButtonNames" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,9 @@
     <sheet name="MktgToolsDropdown URLs" sheetId="5" r:id="rId8"/>
     <sheet name="HelpDropdown Names" sheetId="10" r:id="rId9"/>
     <sheet name="HelpDropdown URLs" sheetId="6" r:id="rId10"/>
+    <sheet name="Location SearchResult Count" sheetId="11" r:id="rId11"/>
+    <sheet name="Location SearchResult Names" sheetId="12" r:id="rId12"/>
+    <sheet name="Location ResultSelect" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Claim Your Listing</t>
   </si>
@@ -129,6 +132,41 @@
   </si>
   <si>
     <t>Owners' Forum</t>
+  </si>
+  <si>
+    <t>New York City
+New York, United States</t>
+  </si>
+  <si>
+    <t>New York
+United States, North America</t>
+  </si>
+  <si>
+    <t>New York Mills
+Minnesota, United States</t>
+  </si>
+  <si>
+    <t>New York Mills
+New York, United States</t>
+  </si>
+  <si>
+    <t>Thousand Islands New York
+New York, United States</t>
+  </si>
+  <si>
+    <t>West New York
+New Jersey, United States</t>
+  </si>
+  <si>
+    <t>New Paltz
+New York, United States</t>
+  </si>
+  <si>
+    <t>New Rochelle
+New York, United States</t>
+  </si>
+  <si>
+    <t>New York City, New York</t>
   </si>
 </sst>
 </file>
@@ -164,8 +202,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,7 +516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -507,6 +548,103 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>

</xml_diff>

<commit_message>
15 Test Cases - TripAdvisor (Owners Page)
</commit_message>
<xml_diff>
--- a/tripAdvisor/src/main/resources/TripAdvisor_OwnersPage_ExpectedElements.xlsx
+++ b/tripAdvisor/src/main/resources/TripAdvisor_OwnersPage_ExpectedElements.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" tabRatio="684" firstSheet="9" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" tabRatio="684" firstSheet="11" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="HeaderBar ButtonNames" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,11 @@
     <sheet name="MktgToolsDropdown URLs" sheetId="5" r:id="rId8"/>
     <sheet name="HelpDropdown Names" sheetId="10" r:id="rId9"/>
     <sheet name="HelpDropdown URLs" sheetId="6" r:id="rId10"/>
-    <sheet name="Location SearchResult Count" sheetId="11" r:id="rId11"/>
+    <sheet name="SearchResult Count" sheetId="11" r:id="rId11"/>
     <sheet name="Location SearchResult Names" sheetId="12" r:id="rId12"/>
     <sheet name="Location ResultSelect" sheetId="13" r:id="rId13"/>
+    <sheet name="BizName SearchResults Names" sheetId="15" r:id="rId14"/>
+    <sheet name="ClaimListingPage Title" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Claim Your Listing</t>
   </si>
@@ -167,6 +169,41 @@
   </si>
   <si>
     <t>New York City, New York</t>
+  </si>
+  <si>
+    <t>The Metropolitan Museum of Art
+1000 5th Ave, New York City, New York</t>
+  </si>
+  <si>
+    <t>The National 9/11 Memorial &amp; Museum
+180 Greenwich St, New York City, New York</t>
+  </si>
+  <si>
+    <t>American Museum of Natural History
+79th Street, New York City, New York</t>
+  </si>
+  <si>
+    <t>The Museum of Modern Art (MoMA)
+11 West 53rd Street, New York City, New York</t>
+  </si>
+  <si>
+    <t>Tenement Museum
+103 Orchard St, New York City, New York</t>
+  </si>
+  <si>
+    <t>Museum of Sex
+233 5th Ave, New York City, New York</t>
+  </si>
+  <si>
+    <t>Intrepid Sea, Air &amp; Space Museum
+12th Avenue &amp; 46th Street, New York City, New York</t>
+  </si>
+  <si>
+    <t>Whitney Museum of American Art
+99 Gansevoort Street, New York City, New York</t>
+  </si>
+  <si>
+    <t>Tripadvisor - Claim Your Listing</t>
   </si>
 </sst>
 </file>
@@ -552,7 +589,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -626,9 +665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -638,6 +675,84 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>